<commit_message>
add hw10 & group gits
</commit_message>
<xml_diff>
--- a/docs/nopublish/groups.xlsx
+++ b/docs/nopublish/groups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnese\Desktop\BRT\Teaching\1_Intro-Data-Science\c1-intro-fall-2022\nopublish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B8528B-8DCA-4207-B91E-8BB4DB5B60FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA84005-4CB4-46FB-834A-10569ABD4400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{4A21B253-F485-4504-8DDC-E700AD6F30FC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{4A21B253-F485-4504-8DDC-E700AD6F30FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
   <si>
     <t>first</t>
   </si>
@@ -228,6 +228,30 @@
   </si>
   <si>
     <t>dstrayer@uoregon.edu</t>
+  </si>
+  <si>
+    <t>https://github.com/seul-b/edld-final</t>
+  </si>
+  <si>
+    <t>in-progress.Rmd</t>
+  </si>
+  <si>
+    <t>https://github.com/haithamanbar/Oregon-made</t>
+  </si>
+  <si>
+    <t>Final Project.Rmd</t>
+  </si>
+  <si>
+    <t>https://github.com/emaduneme/EDLD_651_Ghana</t>
+  </si>
+  <si>
+    <t>https://github.com/tianwalker44/EDLD_Final</t>
+  </si>
+  <si>
+    <t>Final_Groupof5.Rmd</t>
+  </si>
+  <si>
+    <t>Main Markdown.Rmd</t>
   </si>
 </sst>
 </file>
@@ -272,10 +296,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -595,12 +618,15 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="23.1328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -620,231 +646,327 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="E7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="E8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="E9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="E10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="E12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="E13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="E14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="E16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -857,8 +979,14 @@
       <c r="D18" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -871,8 +999,14 @@
       <c r="D19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="C20" s="1"/>
     </row>
   </sheetData>
@@ -897,5 +1031,6 @@
     <hyperlink ref="C15" r:id="rId18" xr:uid="{80422A56-8EBC-4279-B4A6-7B1D8ADEC518}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>